<commit_message>
Function for inserting the excel mapped data into the mongo table assembked..
</commit_message>
<xml_diff>
--- a/uploads/social-card.xlsx
+++ b/uploads/social-card.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t xml:space="preserve">name_child</t>
   </si>
@@ -215,24 +215,6 @@
   </si>
   <si>
     <t xml:space="preserve">residentialBuilding_family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name_familyMember</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jmbg_familyMember</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relationToChild_familyMember</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name_familyMemberTwo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jmbg_familyMemberTwo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relationToChild_familyMemberTwo</t>
   </si>
   <si>
     <t xml:space="preserve">Miki</t>
@@ -340,7 +322,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,12 +411,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0066CC"/>
         <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -472,7 +448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -537,7 +513,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -546,6 +522,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -583,7 +563,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFCCFF00"/>
@@ -629,85 +609,84 @@
   <dimension ref="A1:BS65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BS9" activeCellId="0" sqref="BS9"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.4037037037037"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.7925925925926"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="23.9111111111111"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="34.4925925925926"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="36.9444444444444"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="45.3703703703704"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="55.0740740740741"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="59.0888888888889"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="26.4592592592593"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="31.162962962963"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="37.8259259259259"/>
-    <col collapsed="false" hidden="false" max="70" min="70" style="0" width="35.6703703703704"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="72" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="25.9666666666667"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="25.0851851851852"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="36.2592592592593"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="38.7074074074074"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="47.6259259259259"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="57.8148148148148"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="62.1296296296296"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="27.7333333333333"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="39.6888888888889"/>
+    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="37.4333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="72" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,46 +882,34 @@
       <c r="BM1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="16" t="s">
-        <v>70</v>
-      </c>
+      <c r="BN1" s="16"/>
+      <c r="BO1" s="16"/>
+      <c r="BP1" s="16"/>
+      <c r="BQ1" s="16"/>
+      <c r="BR1" s="16"/>
+      <c r="BS1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" s="17" t="n">
         <v>2039343493</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H2" s="18" t="n">
         <v>72000</v>
@@ -957,37 +924,37 @@
         <v>1</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="O2" s="17" t="n">
         <v>2</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="17" t="n">
         <v>211945112344</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="U2" s="17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="W2" s="17" t="n">
         <v>71000</v>
@@ -1002,34 +969,34 @@
         <v>1</v>
       </c>
       <c r="AA2" s="17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AC2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AD2" s="17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AE2" s="17" t="n">
         <v>33</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AG2" s="17" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AI2" s="17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="AJ2" s="17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="AK2" s="17" t="n">
         <v>71000</v>
@@ -1044,98 +1011,86 @@
         <v>1</v>
       </c>
       <c r="AO2" s="17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AP2" s="17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AQ2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AR2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AS2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AT2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AU2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AV2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AW2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AX2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AY2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AZ2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BA2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BB2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BC2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BD2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BE2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BF2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BG2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BH2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BI2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BJ2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BK2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BL2" s="17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="BM2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="BN2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="BO2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="BP2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="BQ2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="BR2" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="BS2" s="17" t="s">
-        <v>86</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="BN2" s="19"/>
+      <c r="BO2" s="19"/>
+      <c r="BP2" s="19"/>
+      <c r="BQ2" s="19"/>
+      <c r="BR2" s="19"/>
+      <c r="BS2" s="19"/>
     </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1048576" s="17" t="n">

</xml_diff>

<commit_message>
Function for inserting the excel mapped data into the mongo table assembked.. the object fully loaded
</commit_message>
<xml_diff>
--- a/uploads/social-card.xlsx
+++ b/uploads/social-card.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="socialCard" sheetId="1" state="visible" r:id="rId2"/>
@@ -448,7 +448,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -511,14 +511,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -608,82 +600,82 @@
   </sheetPr>
   <dimension ref="A1:BS65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1048544" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1048576" activeCellId="0" sqref="A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.5333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="25.9666666666667"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="36.2592592592593"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="23.9111111111111"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="39.2962962962963"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="38.7074074074074"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="47.6259259259259"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="57.8148148148148"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="62.1296296296296"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="29.8888888888889"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="27.7333333333333"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="32.6333333333333"/>
-    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="39.6888888888889"/>
-    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="72" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.3185185185185"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.362962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="25.6740740740741"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="37.237037037037"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="24.5"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="39.6888888888889"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="48.8"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="59.2851851851852"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="63.6962962962963"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="28.4185185185185"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="33.4148148148148"/>
+    <col collapsed="false" hidden="false" max="69" min="69" style="0" width="40.6666666666667"/>
+    <col collapsed="false" hidden="false" max="71" min="70" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="72" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,7 +903,7 @@
       <c r="G2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="18" t="n">
+      <c r="H2" s="16" t="n">
         <v>72000</v>
       </c>
       <c r="I2" s="17" t="n">
@@ -1085,295 +1077,14 @@
       <c r="BM2" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="BN2" s="19"/>
-      <c r="BO2" s="19"/>
-      <c r="BP2" s="19"/>
-      <c r="BQ2" s="19"/>
-      <c r="BR2" s="19"/>
-      <c r="BS2" s="19"/>
+      <c r="BN2" s="17"/>
+      <c r="BO2" s="17"/>
+      <c r="BP2" s="17"/>
+      <c r="BQ2" s="17"/>
+      <c r="BR2" s="17"/>
+      <c r="BS2" s="17"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1048576" s="17" t="n">
-        <f aca="false">SUM(B2:B1048575)</f>
-        <v>2039343493</v>
-      </c>
-      <c r="C1048576" s="17" t="n">
-        <f aca="false">SUM(C2:C1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="D1048576" s="17" t="n">
-        <f aca="false">SUM(D2:D1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="E1048576" s="17" t="n">
-        <f aca="false">SUM(E2:E1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="F1048576" s="17" t="n">
-        <f aca="false">SUM(F2:F1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="G1048576" s="17" t="n">
-        <f aca="false">SUM(G2:G1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="H1048576" s="17" t="n">
-        <f aca="false">SUM(H2:H1048575)</f>
-        <v>72000</v>
-      </c>
-      <c r="I1048576" s="17" t="n">
-        <f aca="false">SUM(I2:I1048575)</f>
-        <v>1</v>
-      </c>
-      <c r="J1048576" s="17" t="n">
-        <f aca="false">SUM(J2:J1048575)</f>
-        <v>1</v>
-      </c>
-      <c r="K1048576" s="17" t="n">
-        <f aca="false">SUM(K2:K1048575)</f>
-        <v>1</v>
-      </c>
-      <c r="L1048576" s="17" t="n">
-        <f aca="false">SUM(L2:L1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="M1048576" s="17" t="n">
-        <f aca="false">SUM(M2:M1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="N1048576" s="17" t="n">
-        <f aca="false">SUM(N2:N1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="O1048576" s="17" t="n">
-        <f aca="false">SUM(O2:O1048575)</f>
-        <v>2</v>
-      </c>
-      <c r="P1048576" s="17" t="n">
-        <f aca="false">SUM(P2:P1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="Q1048576" s="17" t="n">
-        <f aca="false">SUM(Q2:Q1048575)</f>
-        <v>211945112344</v>
-      </c>
-      <c r="R1048576" s="17" t="n">
-        <f aca="false">SUM(R2:R1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="S1048576" s="17" t="n">
-        <f aca="false">SUM(S2:S1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="T1048576" s="17" t="n">
-        <f aca="false">SUM(T2:T1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="U1048576" s="17" t="n">
-        <f aca="false">SUM(U2:U1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="V1048576" s="17" t="n">
-        <f aca="false">SUM(V2:V1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="W1048576" s="17" t="n">
-        <f aca="false">SUM(W2:W1048575)</f>
-        <v>71000</v>
-      </c>
-      <c r="X1048576" s="17" t="n">
-        <f aca="false">SUM(X2:X1048575)</f>
-        <v>65123333</v>
-      </c>
-      <c r="Y1048576" s="17" t="n">
-        <f aca="false">SUM(Y2:Y1048575)</f>
-        <v>65111333</v>
-      </c>
-      <c r="Z1048576" s="17" t="n">
-        <f aca="false">SUM(Z2:Z1048575)</f>
-        <v>1</v>
-      </c>
-      <c r="AA1048576" s="17" t="n">
-        <f aca="false">SUM(AA2:AA1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AB1048576" s="17" t="n">
-        <f aca="false">SUM(AB2:AB1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AC1048576" s="17" t="n">
-        <f aca="false">SUM(AC2:AC1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AD1048576" s="17" t="n">
-        <f aca="false">SUM(AD2:AD1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AE1048576" s="17" t="n">
-        <f aca="false">SUM(AE2:AE1048575)</f>
-        <v>33</v>
-      </c>
-      <c r="AF1048576" s="17" t="n">
-        <f aca="false">SUM(AF2:AF1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AG1048576" s="17" t="n">
-        <f aca="false">SUM(AG2:AG1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AH1048576" s="17" t="n">
-        <f aca="false">SUM(AH2:AH1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AI1048576" s="17" t="n">
-        <f aca="false">SUM(AI2:AI1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ1048576" s="17" t="n">
-        <f aca="false">SUM(AJ2:AJ1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AK1048576" s="17" t="n">
-        <f aca="false">SUM(AK2:AK1048575)</f>
-        <v>71000</v>
-      </c>
-      <c r="AL1048576" s="17" t="n">
-        <f aca="false">SUM(AL2:AL1048575)</f>
-        <v>65122333</v>
-      </c>
-      <c r="AM1048576" s="17" t="n">
-        <f aca="false">SUM(AM2:AM1048575)</f>
-        <v>65131333</v>
-      </c>
-      <c r="AN1048576" s="17" t="n">
-        <f aca="false">SUM(AN2:AN1048575)</f>
-        <v>1</v>
-      </c>
-      <c r="AO1048576" s="17" t="n">
-        <f aca="false">SUM(AO2:AO1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AP1048576" s="17" t="n">
-        <f aca="false">SUM(AP2:AP1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ1048576" s="17" t="n">
-        <f aca="false">SUM(AQ2:AQ1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AR1048576" s="17" t="n">
-        <f aca="false">SUM(AR2:AR1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AS1048576" s="17" t="n">
-        <f aca="false">SUM(AS2:AS1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AT1048576" s="17" t="n">
-        <f aca="false">SUM(AT2:AT1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AU1048576" s="17" t="n">
-        <f aca="false">SUM(AU2:AU1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AV1048576" s="17" t="n">
-        <f aca="false">SUM(AV2:AV1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AW1048576" s="17" t="n">
-        <f aca="false">SUM(AW2:AW1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AX1048576" s="17" t="n">
-        <f aca="false">SUM(AX2:AX1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AY1048576" s="17" t="n">
-        <f aca="false">SUM(AY2:AY1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ1048576" s="17" t="n">
-        <f aca="false">SUM(AZ2:AZ1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BA1048576" s="17" t="n">
-        <f aca="false">SUM(BA2:BA1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BB1048576" s="17" t="n">
-        <f aca="false">SUM(BB2:BB1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BC1048576" s="17" t="n">
-        <f aca="false">SUM(BC2:BC1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BD1048576" s="17" t="n">
-        <f aca="false">SUM(BD2:BD1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BE1048576" s="17" t="n">
-        <f aca="false">SUM(BE2:BE1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BF1048576" s="17" t="n">
-        <f aca="false">SUM(BF2:BF1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BG1048576" s="17" t="n">
-        <f aca="false">SUM(BG2:BG1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BH1048576" s="17" t="n">
-        <f aca="false">SUM(BH2:BH1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BI1048576" s="17" t="n">
-        <f aca="false">SUM(BI2:BI1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ1048576" s="17" t="n">
-        <f aca="false">SUM(BJ2:BJ1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BK1048576" s="17" t="n">
-        <f aca="false">SUM(BK2:BK1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BL1048576" s="17" t="n">
-        <f aca="false">SUM(BL2:BL1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BM1048576" s="17" t="n">
-        <f aca="false">SUM(BM2:BM1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BN1048576" s="17" t="n">
-        <f aca="false">SUM(BN2:BN1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BO1048576" s="17" t="n">
-        <f aca="false">SUM(BO2:BO1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BP1048576" s="17" t="n">
-        <f aca="false">SUM(BP2:BP1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ1048576" s="17" t="n">
-        <f aca="false">SUM(BQ2:BQ1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BR1048576" s="17" t="n">
-        <f aca="false">SUM(BR2:BR1048575)</f>
-        <v>0</v>
-      </c>
-      <c r="BS1048576" s="17" t="n">
-        <f aca="false">SUM()</f>
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Insert of social card done, functions complete and working
</commit_message>
<xml_diff>
--- a/uploads/social-card.xlsx
+++ b/uploads/social-card.xlsx
@@ -81,40 +81,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="BN1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Family member</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BQ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Family member</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t xml:space="preserve">name_child</t>
   </si>
@@ -161,115 +133,154 @@
     <t xml:space="preserve">healthState_child</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jmbg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">citizenId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">issuedBy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">municipality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">working</t>
-  </si>
-  <si>
-    <t xml:space="preserve">position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qualifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nameOfEmployer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meritalStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chronicalDecease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chronicalDeceaseText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disabilityText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specialNeeds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">familyRelations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incomeBySalary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incomeBySalaryText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">familyPension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">familyPensionText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unemploymentBenefit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unemploymentBenefitText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disabilityCompensation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disabilityCompensationText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compensationForTheSocialProtectionSystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compensationForTheSocialProtectionSystemText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otherIncome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otherIncomeText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">familyResidence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">housingConditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relationToChild</t>
+    <t xml:space="preserve">name_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmbg_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citizenId_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">issuedBy_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">municipality_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postNumber_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tel_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mob_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qualifications_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nameOfEmployer_mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jmbg_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citizenId_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">issuedBy_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">municipality_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postNumber_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tel_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mob_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qualifications_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nameOfEmployer_father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meritalStatus_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chronicalDecease_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chronicalDeceaseText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disability_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disabilityText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specialNeeds_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">familyRelations_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incomeBySalary_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incomeBySalaryText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">familyPension_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">familyPensionText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unemploymentBenefit_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unemploymentBenefitText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disabilityCompensation_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disabilityCompensationText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compensationForTheSocialProtectionSystem_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compensationForTheSocialProtectionSystemText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otherIncome_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otherIncomeText_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">familyResidence_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">housingConditions_family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialBuilding_family</t>
   </si>
   <si>
     <t xml:space="preserve">Miki</t>
@@ -377,7 +388,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,12 +479,6 @@
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -509,7 +514,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,15 +579,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,7 +621,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFCCFF00"/>
@@ -665,70 +666,77 @@
   </sheetPr>
   <dimension ref="A1:BS65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP12" activeCellId="0" sqref="AP12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5592592592593"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.6222222222222"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="27" min="24" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="41" min="30" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="28.2222222222222"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="47.4296296296296"/>
-    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="53.5037037037037"/>
-    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="23.1259259259259"/>
-    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="70" min="69" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="72" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.637037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="27" min="24" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="32" min="30" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="36" min="34" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="11.1703703703704"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="23.4222222222222"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="11.7592592592593"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="27.6333333333333"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="59" min="59" style="0" width="49.7814814814815"/>
+    <col collapsed="false" hidden="false" max="60" min="60" style="0" width="56.2481481481481"/>
+    <col collapsed="false" hidden="false" max="61" min="61" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="62" min="62" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="0" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="64" min="64" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="65" min="65" style="0" width="29.0074074074074"/>
+    <col collapsed="false" hidden="false" max="66" min="66" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="67" min="67" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="70" min="69" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="71" min="71" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="72" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,155 +825,143 @@
         <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="AI1" s="6" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="AL1" s="5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="AM1" s="10" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="AN1" s="11" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="AO1" s="12" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="AP1" s="13" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="AQ1" s="14" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="AR1" s="9" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="AS1" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="AT1" s="10" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="AU1" s="11" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="AV1" s="12" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="AW1" s="4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="AX1" s="6" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="AY1" s="6" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="AZ1" s="7" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="BA1" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="BB1" s="4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="BC1" s="6" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="BD1" s="6" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="BE1" s="7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="BF1" s="4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="BG1" s="7" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="BH1" s="4" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="BI1" s="4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="BJ1" s="15" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="BK1" s="6" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="BL1" s="7" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="BM1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="BO1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="BP1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="BQ1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="BR1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="BS1" s="16" t="s">
-        <v>51</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="BN1" s="16"/>
+      <c r="BO1" s="16"/>
+      <c r="BP1" s="16"/>
+      <c r="BQ1" s="16"/>
+      <c r="BR1" s="16"/>
+      <c r="BS1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B2" s="17" t="n">
         <v>2039343493</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="18" t="n">
+        <v>68</v>
+      </c>
+      <c r="H2" s="16" t="n">
         <v>72000</v>
       </c>
       <c r="I2" s="17" t="n">
@@ -978,37 +974,37 @@
         <v>1</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="O2" s="17" t="n">
         <v>2</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="17" t="n">
         <v>211945112344</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="U2" s="17" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="W2" s="17" t="n">
         <v>71000</v>
@@ -1023,34 +1019,34 @@
         <v>1</v>
       </c>
       <c r="AA2" s="17" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="AC2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AD2" s="17" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="AE2" s="17" t="n">
         <v>33</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="AG2" s="17" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="AI2" s="17" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="AJ2" s="17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="AK2" s="17" t="n">
         <v>71000</v>
@@ -1065,98 +1061,86 @@
         <v>1</v>
       </c>
       <c r="AO2" s="17" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="AP2" s="17" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="AQ2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="AR2" s="17" t="n">
+        <v>0</v>
       </c>
       <c r="AS2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AT2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AU2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AV2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AW2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="AX2" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="AY2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="AZ2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BA2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BB2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BC2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BD2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BE2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BF2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BG2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BH2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BI2" s="17" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="BJ2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BL2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BM2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BN2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BO2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BP2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BR2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BS2" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="BK2" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL2" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="17"/>
+      <c r="BO2" s="17"/>
+      <c r="BP2" s="17"/>
+      <c r="BQ2" s="17"/>
+      <c r="BR2" s="17"/>
+      <c r="BS2" s="17"/>
     </row>
     <row r="1046889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>